<commit_message>
kustutasin whitespace'i ja panin üle ka ühe rea plokke et kaamera katki ei läheks
</commit_message>
<xml_diff>
--- a/jiko.xlsx
+++ b/jiko.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ArgoP\project-Jiko\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karla\project-Jiko\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FFD20B-F0FE-4F0A-AE3A-4ADFB82E7DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2766C7A-AAA0-4C79-B5D9-9BAEA04970E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31230" yWindow="1380" windowWidth="21285" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="38700" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -129,9 +129,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -169,7 +169,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -275,7 +275,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -417,7 +417,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -428,7 +428,7 @@
   <dimension ref="A1:AN40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BE10" sqref="BE10"/>
+      <selection activeCell="BE5" sqref="BE5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,118 +442,118 @@
         <v>1</v>
       </c>
       <c r="B1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN1" s="1">
         <v>1</v>

</xml_diff>